<commit_message>
ozon fix 30.09 part 3
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278C92F1-DDED-534A-8180-8F66AB985A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6888A247-39B3-E14E-8E3D-E8B68F0FE38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="1580" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
+    <workbookView xWindow="9960" yWindow="1760" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -52,13 +52,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +72,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -120,13 +126,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -543,19 +549,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D67642C-E0A6-4DE4-8C14-031D4C3FE90E}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -571,76 +577,311 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>2009921</v>
-      </c>
-      <c r="B2" s="4">
-        <v>161361</v>
-      </c>
-      <c r="C2" s="6">
-        <v>-7</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="A2" s="8">
+        <v>1999960</v>
+      </c>
+      <c r="B2" s="7">
+        <v>228600</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5">
         <v>3.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E3"/>
+      <c r="A3" s="8">
+        <v>2003561</v>
+      </c>
+      <c r="B3" s="7">
+        <v>11563</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E4"/>
+      <c r="A4" s="9">
+        <v>2003597</v>
+      </c>
+      <c r="B4" s="7">
+        <v>51775</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E5"/>
+      <c r="A5" s="9">
+        <v>2003617</v>
+      </c>
+      <c r="B5" s="7">
+        <v>41522</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E6"/>
+      <c r="A6" s="9">
+        <v>2009830</v>
+      </c>
+      <c r="B6" s="7">
+        <v>284287</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E7"/>
+      <c r="A7" s="9">
+        <v>2009879</v>
+      </c>
+      <c r="B7" s="7">
+        <v>15085</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E8"/>
+      <c r="A8" s="9">
+        <v>2009917</v>
+      </c>
+      <c r="B8" s="7">
+        <v>35539</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E9"/>
+      <c r="A9" s="9">
+        <v>2009969</v>
+      </c>
+      <c r="B9" s="7">
+        <v>227168</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E10"/>
+      <c r="A10" s="9">
+        <v>2015327</v>
+      </c>
+      <c r="B10" s="7">
+        <v>147072</v>
+      </c>
+      <c r="C10" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E11"/>
+      <c r="A11" s="9">
+        <v>2021605</v>
+      </c>
+      <c r="B11" s="7">
+        <v>10594</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E12"/>
+      <c r="A12" s="9">
+        <v>2030166</v>
+      </c>
+      <c r="B12" s="7">
+        <v>32436</v>
+      </c>
+      <c r="C12" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E13"/>
+      <c r="A13" s="9">
+        <v>2035584</v>
+      </c>
+      <c r="B13" s="7">
+        <v>83107</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E14"/>
+      <c r="A14" s="9">
+        <v>2037635</v>
+      </c>
+      <c r="B14" s="7">
+        <v>25464</v>
+      </c>
+      <c r="C14" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>2037652</v>
+      </c>
+      <c r="B15" s="7">
+        <v>31203</v>
+      </c>
+      <c r="C15" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>2039689</v>
+      </c>
+      <c r="B16" s="7">
+        <v>262668</v>
+      </c>
+      <c r="C16" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>2039819</v>
+      </c>
+      <c r="B17" s="7">
+        <v>18259</v>
+      </c>
+      <c r="C17" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E18"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="9" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="28"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="30"/>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="9" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="40"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ozon fixes 03.09.25 part 1
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8469D192-AEBD-454E-AB5D-523C5AE451E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67E2E19-26DB-E442-A3B9-141D4DF2EC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="1760" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -552,7 +552,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,10 +583,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
-        <v>1999960</v>
+        <v>2021662</v>
       </c>
       <c r="B2" s="7">
-        <v>147072</v>
+        <v>82253</v>
       </c>
       <c r="C2" s="3">
         <v>-7</v>

</xml_diff>

<commit_message>
ozon fixes 14.10.2025 part 1
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67E2E19-26DB-E442-A3B9-141D4DF2EC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF92E09-3111-9647-A419-CB00773AEE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="1760" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -552,7 +552,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,13 +583,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
-        <v>2021662</v>
+        <v>2071139</v>
       </c>
       <c r="B2" s="7">
-        <v>82253</v>
+        <v>26517</v>
       </c>
       <c r="C2" s="3">
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
ozon fixes 14.10.2025 part 3
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF92E09-3111-9647-A419-CB00773AEE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF229752-DDD1-5A42-8F8C-41B25717D824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="1760" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -552,7 +552,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,10 +583,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
-        <v>2071139</v>
+        <v>2052980</v>
       </c>
       <c r="B2" s="7">
-        <v>26517</v>
+        <v>16360</v>
       </c>
       <c r="C2" s="3">
         <v>-5</v>

</xml_diff>

<commit_message>
ozon fixes 14.10.2025 part 5
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF229752-DDD1-5A42-8F8C-41B25717D824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645E9014-F942-534D-988A-140A90361956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="1760" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -552,7 +552,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -583,13 +583,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
-        <v>2052980</v>
+        <v>2048420</v>
       </c>
       <c r="B2" s="7">
-        <v>16360</v>
+        <v>173518</v>
       </c>
       <c r="C2" s="3">
-        <v>-5</v>
+        <v>-7.5</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
ozon fixes 16.09.2025 part 1
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED09162-646A-2344-9B9D-8F2FF3B39312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CF90B1-82E0-634D-A9E0-0112871A496B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9960" yWindow="1760" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -97,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,12 +108,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -152,7 +146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -168,7 +162,6 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -588,7 +581,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -619,10 +612,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
-        <v>2059029</v>
+        <v>1988393</v>
       </c>
       <c r="B2" s="7">
-        <v>22673</v>
+        <v>44165</v>
       </c>
       <c r="C2" s="3">
         <v>-7</v>
@@ -635,11 +628,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
-        <v>2065794</v>
+      <c r="A3">
+        <v>1999934</v>
       </c>
       <c r="B3" s="7">
-        <v>51850</v>
+        <v>95656</v>
       </c>
       <c r="C3" s="3">
         <v>-7</v>
@@ -652,11 +645,11 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
-        <v>2068125</v>
+      <c r="A4">
+        <v>1999982</v>
       </c>
       <c r="B4" s="10">
-        <v>48512</v>
+        <v>51980</v>
       </c>
       <c r="C4" s="3">
         <v>-7</v>
@@ -669,18 +662,38 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
+      <c r="A5">
+        <v>2012994</v>
+      </c>
+      <c r="B5" s="7">
+        <v>37976</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5"/>
+      <c r="A6">
+        <v>2045531</v>
+      </c>
+      <c r="B6" s="7">
+        <v>19136</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
@@ -775,7 +788,7 @@
       <c r="E22"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A3">
+  <conditionalFormatting sqref="A2">
     <cfRule type="duplicateValues" dxfId="9" priority="31"/>
     <cfRule type="duplicateValues" dxfId="8" priority="32"/>
     <cfRule type="duplicateValues" dxfId="7" priority="33"/>

</xml_diff>

<commit_message>
ozon fixes 30.10.2025 part 3
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1075F4D4-7F64-7649-BC9D-2D7341FF2A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A457DAD-0978-1545-96CD-5A50097A5476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8920" yWindow="1760" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +77,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,9 +151,11 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -479,7 +474,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -510,39 +505,71 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2083871</v>
-      </c>
-      <c r="B2" s="9">
-        <v>25646</v>
+        <v>2083885</v>
+      </c>
+      <c r="B2" s="11">
+        <v>168918</v>
       </c>
       <c r="C2" s="3">
+        <v>7</v>
+      </c>
+      <c r="D2" s="9">
         <v>0</v>
       </c>
-      <c r="D2" s="10">
+      <c r="E2" s="10">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2089334</v>
+      </c>
+      <c r="B3" s="11">
+        <v>16392</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9">
         <v>0</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E3" s="10">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2093685</v>
+      </c>
+      <c r="B4" s="7">
+        <v>52719</v>
+      </c>
+      <c r="C4" s="3">
+        <v>7</v>
+      </c>
+      <c r="D4" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="7"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="7"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="10">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="8">
+        <v>2101450</v>
+      </c>
+      <c r="B5" s="7">
+        <v>58407</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>

</xml_diff>

<commit_message>
brg fixes 10.11.2025 part 2
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80823FF6-3AE1-A545-8465-C1FBF4F1D311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C5C0B6-8425-6741-8E31-0ED8AEA71908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8920" yWindow="1760" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
+    <workbookView xWindow="7100" yWindow="1280" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,13 +72,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -139,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -149,19 +142,120 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -471,16 +565,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D67642C-E0A6-4DE4-8C14-031D4C3FE90E}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" style="6" customWidth="1"/>
@@ -504,118 +598,324 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>2156997</v>
+      <c r="A2" s="9">
+        <v>2060237</v>
       </c>
       <c r="B2" s="11">
-        <v>1000000</v>
+        <v>534990</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9">
-        <v>0</v>
-      </c>
-      <c r="E2" s="10">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
-        <v>2168625</v>
-      </c>
-      <c r="B3" s="11">
-        <v>999990</v>
+      <c r="A3" s="10">
+        <v>2065752</v>
+      </c>
+      <c r="B3" s="3">
+        <v>484484</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="9">
+        <v>2067641</v>
+      </c>
+      <c r="B4" s="11">
+        <v>593991</v>
+      </c>
+      <c r="C4" s="3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="10">
+        <v>2069254</v>
+      </c>
+      <c r="B5" s="3">
+        <v>694990</v>
+      </c>
+      <c r="C5" s="3">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="9">
+        <v>2082359</v>
+      </c>
+      <c r="B6" s="11">
+        <v>659000</v>
+      </c>
+      <c r="C6" s="3">
+        <v>11</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>133</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="10">
+        <v>2086263</v>
+      </c>
+      <c r="B7" s="3">
+        <v>489990</v>
+      </c>
+      <c r="C7" s="3">
+        <v>11</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="9">
+        <v>2099197</v>
+      </c>
+      <c r="B8" s="11">
+        <v>170382</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="10">
+        <v>2102943</v>
+      </c>
+      <c r="B9" s="3">
+        <v>428890</v>
+      </c>
+      <c r="C9" s="3">
+        <v>11</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="9">
+        <v>2104415</v>
+      </c>
+      <c r="B10" s="11">
+        <v>267801</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
+      <c r="A11" s="10">
+        <v>2106429</v>
+      </c>
+      <c r="B11" s="3">
+        <v>684990</v>
+      </c>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <v>13.5</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="5"/>
+      <c r="A12" s="9">
+        <v>2107298</v>
+      </c>
+      <c r="B12" s="11">
+        <v>178402</v>
+      </c>
+      <c r="C12" s="3">
+        <v>10</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E13"/>
+      <c r="A13" s="10">
+        <v>2111413</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1141531</v>
+      </c>
+      <c r="C13" s="12">
+        <v>10</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="13">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E14"/>
+      <c r="A14" s="9">
+        <v>2115832</v>
+      </c>
+      <c r="B14" s="11">
+        <v>148451</v>
+      </c>
+      <c r="C14" s="12">
+        <v>10</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="13">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E15"/>
+      <c r="A15" s="10">
+        <v>2117476</v>
+      </c>
+      <c r="B15" s="3">
+        <v>134309</v>
+      </c>
+      <c r="C15" s="12">
+        <v>10</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E16"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17"/>
+      <c r="A16" s="9">
+        <v>2120482</v>
+      </c>
+      <c r="B16" s="11">
+        <v>377709</v>
+      </c>
+      <c r="C16" s="12">
+        <v>10</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>2126707</v>
+      </c>
+      <c r="B17" s="3">
+        <v>443755</v>
+      </c>
+      <c r="C17" s="12">
+        <v>10</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>2127270</v>
+      </c>
+      <c r="B18" s="11">
+        <v>149194</v>
+      </c>
+      <c r="C18" s="12">
+        <v>10</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0</v>
+      </c>
+      <c r="E18" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>2133879</v>
+      </c>
+      <c r="B19" s="3">
+        <v>155949</v>
+      </c>
+      <c r="C19" s="12">
+        <v>10</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0</v>
+      </c>
+      <c r="E19" s="13">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A9">
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
ozon fixes 14.11.2025 part 1
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DACE4B-5D12-8143-9B2B-E6BA9220003A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA81548E-4626-5348-AF07-0A7F6A107522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2260" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -265,9 +265,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,7 +305,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -411,7 +411,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,7 +553,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,7 +564,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -595,19 +595,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
-        <v>2177602</v>
+        <v>2082359</v>
       </c>
       <c r="B2" s="9">
-        <v>11931</v>
+        <v>659000</v>
       </c>
       <c r="C2" s="3">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" s="6">
         <v>0</v>
       </c>
       <c r="E2" s="7">
-        <v>3.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
ozon fixes 14.11.2025 part 2
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA81548E-4626-5348-AF07-0A7F6A107522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356F0701-1D9E-7C49-B5BE-BBB9EA440A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2260" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -564,7 +564,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -595,19 +595,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
-        <v>2082359</v>
+        <v>2187390</v>
       </c>
       <c r="B2" s="9">
-        <v>659000</v>
+        <v>440000</v>
       </c>
       <c r="C2" s="3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D2" s="6">
         <v>0</v>
       </c>
       <c r="E2" s="7">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
ozon fixes 18.11.25 part 3
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F68D756-8BDF-BE48-A811-535ABA7318F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F015ECC6-996F-5144-872C-8E09D8E2C734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="2260" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -561,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D67642C-E0A6-4DE4-8C14-031D4C3FE90E}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -595,10 +595,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2083871</v>
+        <v>2148226</v>
       </c>
       <c r="B2" s="8">
-        <v>25646</v>
+        <v>78181</v>
       </c>
       <c r="C2" s="3">
         <v>7</v>
@@ -612,10 +612,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2133780</v>
+        <v>2159417</v>
       </c>
       <c r="B3" s="9">
-        <v>28379</v>
+        <v>58395</v>
       </c>
       <c r="C3" s="3">
         <v>7</v>
@@ -628,16 +628,157 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E4"/>
+      <c r="A4">
+        <v>2159872</v>
+      </c>
+      <c r="B4" s="9">
+        <v>112094</v>
+      </c>
+      <c r="C4" s="3">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E5"/>
+      <c r="A5">
+        <v>2164252</v>
+      </c>
+      <c r="B5" s="9">
+        <v>41551</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E6"/>
+      <c r="A6">
+        <v>2168432</v>
+      </c>
+      <c r="B6" s="9">
+        <v>25581</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E7"/>
+      <c r="A7">
+        <v>2177621</v>
+      </c>
+      <c r="B7" s="9">
+        <v>87923</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2181725</v>
+      </c>
+      <c r="B8" s="9">
+        <v>30916</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2181750</v>
+      </c>
+      <c r="B9" s="9">
+        <v>28931</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2185057</v>
+      </c>
+      <c r="B10" s="9">
+        <v>73218</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2188687</v>
+      </c>
+      <c r="B11" s="9">
+        <v>49081</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2188702</v>
+      </c>
+      <c r="B12" s="9">
+        <v>125119</v>
+      </c>
+      <c r="C12" s="3">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ozon fixes 02.12.2025 part 1
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2022DECC-A0E0-594A-A5C0-11A6ECF46EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913E0738-84F0-194E-8154-347D7925FF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7800" yWindow="1940" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -481,7 +481,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -512,173 +512,89 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
-        <v>2099197</v>
+        <v>2251357</v>
       </c>
       <c r="B2" s="7">
-        <v>170382</v>
+        <v>20738</v>
       </c>
       <c r="C2" s="3">
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="D2" s="6">
         <v>0</v>
       </c>
       <c r="E2" s="6">
-        <v>10.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
-        <v>2104415</v>
+        <v>2250143</v>
       </c>
       <c r="B3" s="8">
-        <v>267801</v>
+        <v>48178</v>
       </c>
       <c r="C3" s="3">
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>10.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
-        <v>2107298</v>
+        <v>2249706</v>
       </c>
       <c r="B4" s="8">
-        <v>178402</v>
+        <v>98411</v>
       </c>
       <c r="C4" s="3">
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
       </c>
       <c r="E4" s="6">
-        <v>10.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
-        <v>2111413</v>
+        <v>2249281</v>
       </c>
       <c r="B5" s="8">
-        <v>1141531</v>
+        <v>17795</v>
       </c>
       <c r="C5" s="3">
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
       </c>
       <c r="E5" s="6">
-        <v>10.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
-        <v>2115832</v>
-      </c>
-      <c r="B6" s="8">
-        <v>148451</v>
-      </c>
-      <c r="C6" s="3">
-        <v>10</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>10.5</v>
-      </c>
+      <c r="E6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
-        <v>2117476</v>
-      </c>
-      <c r="B7" s="8">
-        <v>134309</v>
-      </c>
-      <c r="C7" s="3">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>10.5</v>
-      </c>
+      <c r="E7"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
-        <v>2120482</v>
-      </c>
-      <c r="B8" s="8">
-        <v>377709</v>
-      </c>
-      <c r="C8" s="3">
-        <v>10</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6">
-        <v>10.5</v>
-      </c>
+      <c r="E8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>2126707</v>
-      </c>
-      <c r="B9" s="8">
-        <v>443755</v>
-      </c>
-      <c r="C9" s="3">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6">
-        <v>10.5</v>
-      </c>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>2127270</v>
-      </c>
-      <c r="B10" s="8">
-        <v>149194</v>
-      </c>
-      <c r="C10" s="3">
-        <v>10</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6">
-        <v>10.5</v>
-      </c>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
-        <v>2133879</v>
-      </c>
-      <c r="B11" s="8">
-        <v>155949</v>
-      </c>
-      <c r="C11" s="3">
-        <v>10</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>10.5</v>
-      </c>
+      <c r="E11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ozon fixes 02.12.2025 part 2
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913E0738-84F0-194E-8154-347D7925FF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2D483B-3DA8-6D46-A51F-7DE53C06B1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7800" yWindow="1940" windowWidth="25640" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>order</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>from_merch</t>
+  </si>
+  <si>
+    <t>129705.00</t>
+  </si>
+  <si>
+    <t>64132.00</t>
+  </si>
+  <si>
+    <t>120337.00</t>
+  </si>
+  <si>
+    <t>11860.00</t>
   </si>
 </sst>
 </file>
@@ -149,7 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -159,10 +171,17 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -481,7 +500,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -511,84 +530,140 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
-        <v>2251357</v>
-      </c>
-      <c r="B2" s="7">
-        <v>20738</v>
+      <c r="A2" s="7">
+        <v>2246759</v>
+      </c>
+      <c r="B2" s="9">
+        <v>465060</v>
       </c>
       <c r="C2" s="3">
-        <v>1.5</v>
+        <v>7</v>
       </c>
       <c r="D2" s="6">
         <v>0</v>
       </c>
       <c r="E2" s="6">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
-        <v>2250143</v>
-      </c>
-      <c r="B3" s="8">
-        <v>48178</v>
+      <c r="A3" s="8">
+        <v>2246576</v>
+      </c>
+      <c r="B3" s="10">
+        <v>307456</v>
       </c>
       <c r="C3" s="3">
-        <v>1.5</v>
+        <v>7</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="E3" s="6">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
-        <v>2249706</v>
-      </c>
-      <c r="B4" s="8">
-        <v>98411</v>
+      <c r="A4" s="7">
+        <v>2239991</v>
+      </c>
+      <c r="B4" s="10">
+        <v>26853</v>
       </c>
       <c r="C4" s="3">
-        <v>1.5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
       </c>
       <c r="E4" s="6">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
-        <v>2249281</v>
-      </c>
-      <c r="B5" s="8">
-        <v>17795</v>
+      <c r="A5" s="8">
+        <v>2236242</v>
+      </c>
+      <c r="B5" s="10">
+        <v>33122</v>
       </c>
       <c r="C5" s="3">
-        <v>1.5</v>
+        <v>7</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
       </c>
       <c r="E5" s="6">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E6"/>
+      <c r="A6">
+        <v>2236236</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E7"/>
+      <c r="A7">
+        <v>2231515</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E8"/>
+      <c r="A8">
+        <v>2202028</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E9"/>
+      <c r="A9">
+        <v>2192371</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E10"/>

</xml_diff>

<commit_message>
ozon fixes 26.12.2025 part 3
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE18B46-0278-C644-ACEF-9535013F6F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3D7D35-020E-4142-81E2-1C91E8749142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2100" windowWidth="13180" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,7 +79,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -97,7 +103,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -127,6 +133,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -137,16 +158,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -563,126 +584,1754 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D67642C-E0A6-4DE4-8C14-031D4C3FE90E}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>2138332</v>
+      <c r="A2" s="6">
+        <v>2185732</v>
       </c>
       <c r="B2" s="9">
-        <v>114740</v>
-      </c>
-      <c r="C2" s="9">
-        <v>0</v>
-      </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2" s="9">
-        <v>3.5</v>
+        <v>900000</v>
+      </c>
+      <c r="C2" s="7">
+        <v>19</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2151818</v>
-      </c>
-      <c r="B3" s="3">
-        <v>142300</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9">
-        <v>3.5</v>
+      <c r="A3" s="6">
+        <v>2187622</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1310000</v>
+      </c>
+      <c r="C3" s="7">
+        <v>19</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2150458</v>
-      </c>
-      <c r="B4" s="3">
-        <v>42943</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9">
-        <v>3.5</v>
+      <c r="A4" s="6">
+        <v>2188497</v>
+      </c>
+      <c r="B4" s="9">
+        <v>580000</v>
+      </c>
+      <c r="C4" s="7">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="9"/>
+      <c r="A5" s="6">
+        <v>2187587</v>
+      </c>
+      <c r="B5" s="9">
+        <v>610000</v>
+      </c>
+      <c r="C5" s="7">
+        <v>19</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="6">
+        <v>2187547</v>
+      </c>
+      <c r="B6" s="9">
+        <v>720000</v>
+      </c>
+      <c r="C6" s="7">
+        <v>19</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="9"/>
+      <c r="A7" s="6">
+        <v>2187947</v>
+      </c>
+      <c r="B7" s="9">
+        <v>980000</v>
+      </c>
+      <c r="C7" s="7">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="6">
+        <v>2188505</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1980000</v>
+      </c>
+      <c r="C8" s="7">
+        <v>19</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="A9" s="6">
+        <v>2191555</v>
+      </c>
+      <c r="B9" s="9">
+        <v>784500</v>
+      </c>
+      <c r="C9" s="7">
+        <v>19</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E10"/>
+      <c r="A10" s="6">
+        <v>2191671</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="C10" s="7">
+        <v>19</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>21</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E11"/>
+      <c r="A11" s="6">
+        <v>2190930</v>
+      </c>
+      <c r="B11" s="9">
+        <v>640000</v>
+      </c>
+      <c r="C11" s="7">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>2190915</v>
+      </c>
+      <c r="B12" s="9">
+        <v>980000</v>
+      </c>
+      <c r="C12" s="7">
+        <v>19</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>2190975</v>
+      </c>
+      <c r="B13" s="9">
+        <v>2000000</v>
+      </c>
+      <c r="C13" s="7">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>2191897</v>
+      </c>
+      <c r="B14" s="9">
+        <v>720000</v>
+      </c>
+      <c r="C14" s="7">
+        <v>19</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>2192105</v>
+      </c>
+      <c r="B15" s="9">
+        <v>764000</v>
+      </c>
+      <c r="C15" s="7">
+        <v>19</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>2192322</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1246300</v>
+      </c>
+      <c r="C16" s="7">
+        <v>19</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>2192427</v>
+      </c>
+      <c r="B17" s="9">
+        <v>840000</v>
+      </c>
+      <c r="C17" s="7">
+        <v>19</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>2192481</v>
+      </c>
+      <c r="B18" s="9">
+        <v>410000</v>
+      </c>
+      <c r="C18" s="7">
+        <v>19</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>2192629</v>
+      </c>
+      <c r="B19" s="9">
+        <v>360000</v>
+      </c>
+      <c r="C19" s="7">
+        <v>19</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>2191699</v>
+      </c>
+      <c r="B20" s="9">
+        <v>500000</v>
+      </c>
+      <c r="C20" s="7">
+        <v>19</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>2191694</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1210000</v>
+      </c>
+      <c r="C21" s="7">
+        <v>19</v>
+      </c>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>2191858</v>
+      </c>
+      <c r="B22" s="9">
+        <v>750000</v>
+      </c>
+      <c r="C22" s="7">
+        <v>19</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>2192459</v>
+      </c>
+      <c r="B23" s="9">
+        <v>1210000</v>
+      </c>
+      <c r="C23" s="7">
+        <v>19</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>2190947</v>
+      </c>
+      <c r="B24" s="9">
+        <v>1100000</v>
+      </c>
+      <c r="C24" s="7">
+        <v>19</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>2191852</v>
+      </c>
+      <c r="B25" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="C25" s="7">
+        <v>19</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>2192593</v>
+      </c>
+      <c r="B26" s="9">
+        <v>1200000</v>
+      </c>
+      <c r="C26" s="7">
+        <v>19</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>2191801</v>
+      </c>
+      <c r="B27" s="9">
+        <v>690000</v>
+      </c>
+      <c r="C27" s="7">
+        <v>19</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>2192372</v>
+      </c>
+      <c r="B28" s="9">
+        <v>850000</v>
+      </c>
+      <c r="C28" s="7">
+        <v>19</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>2196051</v>
+      </c>
+      <c r="B29" s="9">
+        <v>336000</v>
+      </c>
+      <c r="C29" s="7">
+        <v>19</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>2195756</v>
+      </c>
+      <c r="B30" s="9">
+        <v>1225000</v>
+      </c>
+      <c r="C30" s="7">
+        <v>19</v>
+      </c>
+      <c r="D30" s="8">
+        <v>0</v>
+      </c>
+      <c r="E30" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>2194373</v>
+      </c>
+      <c r="B31" s="9">
+        <v>490000</v>
+      </c>
+      <c r="C31" s="7">
+        <v>19</v>
+      </c>
+      <c r="D31" s="8">
+        <v>0</v>
+      </c>
+      <c r="E31" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>2195684</v>
+      </c>
+      <c r="B32" s="9">
+        <v>845000</v>
+      </c>
+      <c r="C32" s="7">
+        <v>19</v>
+      </c>
+      <c r="D32" s="8">
+        <v>0</v>
+      </c>
+      <c r="E32" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
+        <v>2196016</v>
+      </c>
+      <c r="B33" s="9">
+        <v>550000</v>
+      </c>
+      <c r="C33" s="7">
+        <v>19</v>
+      </c>
+      <c r="D33" s="8">
+        <v>0</v>
+      </c>
+      <c r="E33" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>2195340</v>
+      </c>
+      <c r="B34" s="9">
+        <v>1700000</v>
+      </c>
+      <c r="C34" s="7">
+        <v>19</v>
+      </c>
+      <c r="D34" s="8">
+        <v>0</v>
+      </c>
+      <c r="E34" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>2194532</v>
+      </c>
+      <c r="B35" s="9">
+        <v>600000</v>
+      </c>
+      <c r="C35" s="7">
+        <v>19</v>
+      </c>
+      <c r="D35" s="8">
+        <v>0</v>
+      </c>
+      <c r="E35" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>2195223</v>
+      </c>
+      <c r="B36" s="9">
+        <v>400000</v>
+      </c>
+      <c r="C36" s="7">
+        <v>19</v>
+      </c>
+      <c r="D36" s="8">
+        <v>0</v>
+      </c>
+      <c r="E36" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>2195530</v>
+      </c>
+      <c r="B37" s="9">
+        <v>500000</v>
+      </c>
+      <c r="C37" s="7">
+        <v>19</v>
+      </c>
+      <c r="D37" s="8">
+        <v>0</v>
+      </c>
+      <c r="E37" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>2197673</v>
+      </c>
+      <c r="B38" s="9">
+        <v>980000</v>
+      </c>
+      <c r="C38" s="7">
+        <v>19</v>
+      </c>
+      <c r="D38" s="8">
+        <v>0</v>
+      </c>
+      <c r="E38" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>2197833</v>
+      </c>
+      <c r="B39" s="9">
+        <v>441000</v>
+      </c>
+      <c r="C39" s="7">
+        <v>19</v>
+      </c>
+      <c r="D39" s="8">
+        <v>0</v>
+      </c>
+      <c r="E39" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="6">
+        <v>2197966</v>
+      </c>
+      <c r="B40" s="9">
+        <v>690000</v>
+      </c>
+      <c r="C40" s="7">
+        <v>19</v>
+      </c>
+      <c r="D40" s="8">
+        <v>0</v>
+      </c>
+      <c r="E40" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="6">
+        <v>2198087</v>
+      </c>
+      <c r="B41" s="9">
+        <v>845000</v>
+      </c>
+      <c r="C41" s="7">
+        <v>19</v>
+      </c>
+      <c r="D41" s="8">
+        <v>0</v>
+      </c>
+      <c r="E41" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="6">
+        <v>2198794</v>
+      </c>
+      <c r="B42" s="9">
+        <v>539000</v>
+      </c>
+      <c r="C42" s="7">
+        <v>19</v>
+      </c>
+      <c r="D42" s="8">
+        <v>0</v>
+      </c>
+      <c r="E42" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="6">
+        <v>2199760</v>
+      </c>
+      <c r="B43" s="9">
+        <v>720000</v>
+      </c>
+      <c r="C43" s="7">
+        <v>19</v>
+      </c>
+      <c r="D43" s="8">
+        <v>0</v>
+      </c>
+      <c r="E43" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="6">
+        <v>2199588</v>
+      </c>
+      <c r="B44" s="9">
+        <v>1500000</v>
+      </c>
+      <c r="C44" s="7">
+        <v>19</v>
+      </c>
+      <c r="D44" s="8">
+        <v>0</v>
+      </c>
+      <c r="E44" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>2201812</v>
+      </c>
+      <c r="B45" s="9">
+        <v>1310000</v>
+      </c>
+      <c r="C45" s="7">
+        <v>19</v>
+      </c>
+      <c r="D45" s="8">
+        <v>0</v>
+      </c>
+      <c r="E45" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
+        <v>2202893</v>
+      </c>
+      <c r="B46" s="9">
+        <v>600000</v>
+      </c>
+      <c r="C46" s="7">
+        <v>19</v>
+      </c>
+      <c r="D46" s="8">
+        <v>0</v>
+      </c>
+      <c r="E46" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>2202444</v>
+      </c>
+      <c r="B47" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="C47" s="7">
+        <v>19</v>
+      </c>
+      <c r="D47" s="8">
+        <v>0</v>
+      </c>
+      <c r="E47" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="6">
+        <v>2202508</v>
+      </c>
+      <c r="B48" s="9">
+        <v>390000</v>
+      </c>
+      <c r="C48" s="7">
+        <v>19</v>
+      </c>
+      <c r="D48" s="8">
+        <v>0</v>
+      </c>
+      <c r="E48" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>2200916</v>
+      </c>
+      <c r="B49" s="9">
+        <v>1210000</v>
+      </c>
+      <c r="C49" s="7">
+        <v>19</v>
+      </c>
+      <c r="D49" s="8">
+        <v>0</v>
+      </c>
+      <c r="E49" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>2202928</v>
+      </c>
+      <c r="B50" s="9">
+        <v>860000</v>
+      </c>
+      <c r="C50" s="7">
+        <v>19</v>
+      </c>
+      <c r="D50" s="8">
+        <v>0</v>
+      </c>
+      <c r="E50" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>2201798</v>
+      </c>
+      <c r="B51" s="9">
+        <v>1110000</v>
+      </c>
+      <c r="C51" s="7">
+        <v>19</v>
+      </c>
+      <c r="D51" s="8">
+        <v>0</v>
+      </c>
+      <c r="E51" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="6">
+        <v>2202362</v>
+      </c>
+      <c r="B52" s="9">
+        <v>453000</v>
+      </c>
+      <c r="C52" s="7">
+        <v>19</v>
+      </c>
+      <c r="D52" s="8">
+        <v>0</v>
+      </c>
+      <c r="E52" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>2204864</v>
+      </c>
+      <c r="B53" s="9">
+        <v>1190000</v>
+      </c>
+      <c r="C53" s="7">
+        <v>19</v>
+      </c>
+      <c r="D53" s="8">
+        <v>0</v>
+      </c>
+      <c r="E53" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="6">
+        <v>2206235</v>
+      </c>
+      <c r="B54" s="9">
+        <v>730000</v>
+      </c>
+      <c r="C54" s="7">
+        <v>19</v>
+      </c>
+      <c r="D54" s="8">
+        <v>0</v>
+      </c>
+      <c r="E54" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
+        <v>2205095</v>
+      </c>
+      <c r="B55" s="9">
+        <v>500000</v>
+      </c>
+      <c r="C55" s="7">
+        <v>19</v>
+      </c>
+      <c r="D55" s="8">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="6">
+        <v>2205366</v>
+      </c>
+      <c r="B56" s="9">
+        <v>850000</v>
+      </c>
+      <c r="C56" s="7">
+        <v>19</v>
+      </c>
+      <c r="D56" s="8">
+        <v>0</v>
+      </c>
+      <c r="E56" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="6">
+        <v>2204976</v>
+      </c>
+      <c r="B57" s="9">
+        <v>690000</v>
+      </c>
+      <c r="C57" s="7">
+        <v>19</v>
+      </c>
+      <c r="D57" s="8">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="6">
+        <v>2206534</v>
+      </c>
+      <c r="B58" s="9">
+        <v>980000</v>
+      </c>
+      <c r="C58" s="7">
+        <v>19</v>
+      </c>
+      <c r="D58" s="8">
+        <v>0</v>
+      </c>
+      <c r="E58" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>2204906</v>
+      </c>
+      <c r="B59" s="9">
+        <v>555000</v>
+      </c>
+      <c r="C59" s="7">
+        <v>19</v>
+      </c>
+      <c r="D59" s="8">
+        <v>0</v>
+      </c>
+      <c r="E59" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="6">
+        <v>2210269</v>
+      </c>
+      <c r="B60" s="9">
+        <v>680000</v>
+      </c>
+      <c r="C60" s="7">
+        <v>19</v>
+      </c>
+      <c r="D60" s="8">
+        <v>0</v>
+      </c>
+      <c r="E60" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="6">
+        <v>2210279</v>
+      </c>
+      <c r="B61" s="9">
+        <v>945000</v>
+      </c>
+      <c r="C61" s="7">
+        <v>19</v>
+      </c>
+      <c r="D61" s="8">
+        <v>0</v>
+      </c>
+      <c r="E61" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="6">
+        <v>2211964</v>
+      </c>
+      <c r="B62" s="9">
+        <v>196000</v>
+      </c>
+      <c r="C62" s="7">
+        <v>19</v>
+      </c>
+      <c r="D62" s="8">
+        <v>0</v>
+      </c>
+      <c r="E62" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
+        <v>2212236</v>
+      </c>
+      <c r="B63" s="9">
+        <v>447860</v>
+      </c>
+      <c r="C63" s="7">
+        <v>19</v>
+      </c>
+      <c r="D63" s="8">
+        <v>0</v>
+      </c>
+      <c r="E63" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="6">
+        <v>2212553</v>
+      </c>
+      <c r="B64" s="9">
+        <v>637200</v>
+      </c>
+      <c r="C64" s="7">
+        <v>19</v>
+      </c>
+      <c r="D64" s="8">
+        <v>0</v>
+      </c>
+      <c r="E64" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="6">
+        <v>2217885</v>
+      </c>
+      <c r="B65" s="9">
+        <v>780000</v>
+      </c>
+      <c r="C65" s="7">
+        <v>19</v>
+      </c>
+      <c r="D65" s="8">
+        <v>0</v>
+      </c>
+      <c r="E65" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="6">
+        <v>2217636</v>
+      </c>
+      <c r="B66" s="9">
+        <v>550000</v>
+      </c>
+      <c r="C66" s="7">
+        <v>19</v>
+      </c>
+      <c r="D66" s="8">
+        <v>0</v>
+      </c>
+      <c r="E66" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>2217871</v>
+      </c>
+      <c r="B67" s="9">
+        <v>330000</v>
+      </c>
+      <c r="C67" s="7">
+        <v>19</v>
+      </c>
+      <c r="D67" s="8">
+        <v>0</v>
+      </c>
+      <c r="E67" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="6">
+        <v>2217242</v>
+      </c>
+      <c r="B68" s="9">
+        <v>720000</v>
+      </c>
+      <c r="C68" s="7">
+        <v>19</v>
+      </c>
+      <c r="D68" s="8">
+        <v>0</v>
+      </c>
+      <c r="E68" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="6">
+        <v>2216202</v>
+      </c>
+      <c r="B69" s="9">
+        <v>1310000</v>
+      </c>
+      <c r="C69" s="7">
+        <v>19</v>
+      </c>
+      <c r="D69" s="8">
+        <v>0</v>
+      </c>
+      <c r="E69" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="6">
+        <v>2219760</v>
+      </c>
+      <c r="B70" s="9">
+        <v>675000</v>
+      </c>
+      <c r="C70" s="7">
+        <v>19</v>
+      </c>
+      <c r="D70" s="8">
+        <v>0</v>
+      </c>
+      <c r="E70" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
+        <v>2220247</v>
+      </c>
+      <c r="B71" s="9">
+        <v>442000</v>
+      </c>
+      <c r="C71" s="7">
+        <v>19</v>
+      </c>
+      <c r="D71" s="8">
+        <v>0</v>
+      </c>
+      <c r="E71" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
+        <v>2220463</v>
+      </c>
+      <c r="B72" s="9">
+        <v>350000</v>
+      </c>
+      <c r="C72" s="7">
+        <v>19</v>
+      </c>
+      <c r="D72" s="8">
+        <v>0</v>
+      </c>
+      <c r="E72" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="6">
+        <v>2221118</v>
+      </c>
+      <c r="B73" s="9">
+        <v>1310000</v>
+      </c>
+      <c r="C73" s="7">
+        <v>19</v>
+      </c>
+      <c r="D73" s="8">
+        <v>0</v>
+      </c>
+      <c r="E73" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="6">
+        <v>2220960</v>
+      </c>
+      <c r="B74" s="9">
+        <v>1200000</v>
+      </c>
+      <c r="C74" s="7">
+        <v>19</v>
+      </c>
+      <c r="D74" s="8">
+        <v>0</v>
+      </c>
+      <c r="E74" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="6">
+        <v>2223277</v>
+      </c>
+      <c r="B75" s="9">
+        <v>980000</v>
+      </c>
+      <c r="C75" s="7">
+        <v>19</v>
+      </c>
+      <c r="D75" s="8">
+        <v>0</v>
+      </c>
+      <c r="E75" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="6">
+        <v>2223822</v>
+      </c>
+      <c r="B76" s="9">
+        <v>899000</v>
+      </c>
+      <c r="C76" s="7">
+        <v>19</v>
+      </c>
+      <c r="D76" s="8">
+        <v>0</v>
+      </c>
+      <c r="E76" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="6">
+        <v>2223803</v>
+      </c>
+      <c r="B77" s="9">
+        <v>540000</v>
+      </c>
+      <c r="C77" s="7">
+        <v>19</v>
+      </c>
+      <c r="D77" s="8">
+        <v>0</v>
+      </c>
+      <c r="E77" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="6">
+        <v>2223589</v>
+      </c>
+      <c r="B78" s="9">
+        <v>890000</v>
+      </c>
+      <c r="C78" s="7">
+        <v>19</v>
+      </c>
+      <c r="D78" s="8">
+        <v>0</v>
+      </c>
+      <c r="E78" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="6">
+        <v>2227183</v>
+      </c>
+      <c r="B79" s="9">
+        <v>1200000</v>
+      </c>
+      <c r="C79" s="7">
+        <v>19</v>
+      </c>
+      <c r="D79" s="8">
+        <v>0</v>
+      </c>
+      <c r="E79" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="6">
+        <v>2228310</v>
+      </c>
+      <c r="B80" s="9">
+        <v>320000</v>
+      </c>
+      <c r="C80" s="7">
+        <v>19</v>
+      </c>
+      <c r="D80" s="8">
+        <v>0</v>
+      </c>
+      <c r="E80" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="6">
+        <v>2228478</v>
+      </c>
+      <c r="B81" s="9">
+        <v>1260000</v>
+      </c>
+      <c r="C81" s="7">
+        <v>19</v>
+      </c>
+      <c r="D81" s="8">
+        <v>0</v>
+      </c>
+      <c r="E81" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="6">
+        <v>2228485</v>
+      </c>
+      <c r="B82" s="9">
+        <v>1100000</v>
+      </c>
+      <c r="C82" s="7">
+        <v>19</v>
+      </c>
+      <c r="D82" s="8">
+        <v>0</v>
+      </c>
+      <c r="E82" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="6">
+        <v>2227662</v>
+      </c>
+      <c r="B83" s="9">
+        <v>476000</v>
+      </c>
+      <c r="C83" s="7">
+        <v>19</v>
+      </c>
+      <c r="D83" s="8">
+        <v>0</v>
+      </c>
+      <c r="E83" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="6">
+        <v>2226933</v>
+      </c>
+      <c r="B84" s="9">
+        <v>562800</v>
+      </c>
+      <c r="C84" s="7">
+        <v>19</v>
+      </c>
+      <c r="D84" s="8">
+        <v>0</v>
+      </c>
+      <c r="E84" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="6">
+        <v>2226620</v>
+      </c>
+      <c r="B85" s="9">
+        <v>1310000</v>
+      </c>
+      <c r="C85" s="7">
+        <v>19</v>
+      </c>
+      <c r="D85" s="8">
+        <v>0</v>
+      </c>
+      <c r="E85" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="6">
+        <v>2228393</v>
+      </c>
+      <c r="B86" s="9">
+        <v>1310000</v>
+      </c>
+      <c r="C86" s="7">
+        <v>19</v>
+      </c>
+      <c r="D86" s="8">
+        <v>0</v>
+      </c>
+      <c r="E86" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="6">
+        <v>2228547</v>
+      </c>
+      <c r="B87" s="9">
+        <v>1310000</v>
+      </c>
+      <c r="C87" s="7">
+        <v>19</v>
+      </c>
+      <c r="D87" s="8">
+        <v>0</v>
+      </c>
+      <c r="E87" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="6">
+        <v>2230435</v>
+      </c>
+      <c r="B88" s="9">
+        <v>589380</v>
+      </c>
+      <c r="C88" s="7">
+        <v>19</v>
+      </c>
+      <c r="D88" s="8">
+        <v>0</v>
+      </c>
+      <c r="E88" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="6">
+        <v>2232021</v>
+      </c>
+      <c r="B89" s="9">
+        <v>720000</v>
+      </c>
+      <c r="C89" s="7">
+        <v>19</v>
+      </c>
+      <c r="D89" s="8">
+        <v>0</v>
+      </c>
+      <c r="E89" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="6">
+        <v>2232197</v>
+      </c>
+      <c r="B90" s="9">
+        <v>1100000</v>
+      </c>
+      <c r="C90" s="7">
+        <v>19</v>
+      </c>
+      <c r="D90" s="8">
+        <v>0</v>
+      </c>
+      <c r="E90" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="6">
+        <v>2231131</v>
+      </c>
+      <c r="B91" s="9">
+        <v>266000</v>
+      </c>
+      <c r="C91" s="7">
+        <v>19</v>
+      </c>
+      <c r="D91" s="8">
+        <v>0</v>
+      </c>
+      <c r="E91" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="6">
+        <v>2231238</v>
+      </c>
+      <c r="B92" s="9">
+        <v>1330000</v>
+      </c>
+      <c r="C92" s="7">
+        <v>19</v>
+      </c>
+      <c r="D92" s="8">
+        <v>0</v>
+      </c>
+      <c r="E92" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="6">
+        <v>2234982</v>
+      </c>
+      <c r="B93" s="9">
+        <v>1200000</v>
+      </c>
+      <c r="C93" s="7">
+        <v>19</v>
+      </c>
+      <c r="D93" s="8">
+        <v>0</v>
+      </c>
+      <c r="E93" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="6">
+        <v>2236095</v>
+      </c>
+      <c r="B94" s="9">
+        <v>1110000</v>
+      </c>
+      <c r="C94" s="7">
+        <v>19</v>
+      </c>
+      <c r="D94" s="8">
+        <v>0</v>
+      </c>
+      <c r="E94" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="6">
+        <v>2235242</v>
+      </c>
+      <c r="B95" s="9">
+        <v>890500</v>
+      </c>
+      <c r="C95" s="7">
+        <v>19</v>
+      </c>
+      <c r="D95" s="8">
+        <v>0</v>
+      </c>
+      <c r="E95" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="6">
+        <v>2238194</v>
+      </c>
+      <c r="B96" s="9">
+        <v>220000</v>
+      </c>
+      <c r="C96" s="7">
+        <v>19</v>
+      </c>
+      <c r="D96" s="8">
+        <v>0</v>
+      </c>
+      <c r="E96" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="6">
+        <v>2241362</v>
+      </c>
+      <c r="B97" s="9">
+        <v>770000</v>
+      </c>
+      <c r="C97" s="7">
+        <v>19</v>
+      </c>
+      <c r="D97" s="8">
+        <v>0</v>
+      </c>
+      <c r="E97" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="6">
+        <v>2242712</v>
+      </c>
+      <c r="B98" s="9">
+        <v>330000</v>
+      </c>
+      <c r="C98" s="7">
+        <v>19</v>
+      </c>
+      <c r="D98" s="8">
+        <v>0</v>
+      </c>
+      <c r="E98" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="6">
+        <v>2241227</v>
+      </c>
+      <c r="B99" s="9">
+        <v>300000</v>
+      </c>
+      <c r="C99" s="7">
+        <v>19</v>
+      </c>
+      <c r="D99" s="8">
+        <v>0</v>
+      </c>
+      <c r="E99" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="6">
+        <v>2242560</v>
+      </c>
+      <c r="B100" s="9">
+        <v>290000</v>
+      </c>
+      <c r="C100" s="7">
+        <v>19</v>
+      </c>
+      <c r="D100" s="8">
+        <v>0</v>
+      </c>
+      <c r="E100" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="6">
+        <v>2245515</v>
+      </c>
+      <c r="B101" s="9">
+        <v>500000</v>
+      </c>
+      <c r="C101" s="7">
+        <v>19</v>
+      </c>
+      <c r="D101" s="8">
+        <v>0</v>
+      </c>
+      <c r="E101" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="6">
+        <v>2244843</v>
+      </c>
+      <c r="B102" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="C102" s="7">
+        <v>19</v>
+      </c>
+      <c r="D102" s="8">
+        <v>0</v>
+      </c>
+      <c r="E102" s="7">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A5">

</xml_diff>

<commit_message>
ozon fixes 15.01.2026 part 1
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9FC360-4F6E-A742-9AAB-F71EDE9B4052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F83A594-F409-AB4D-8288-5434A20B442D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2500" windowWidth="13180" windowHeight="12520" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
+    <workbookView xWindow="2240" yWindow="1040" windowWidth="27580" windowHeight="13980" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -147,12 +147,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -169,6 +180,10 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -588,7 +603,7 @@
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -618,429 +633,329 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>2139527</v>
-      </c>
-      <c r="B2" s="2">
-        <v>59360</v>
-      </c>
-      <c r="C2" s="4">
-        <v>7</v>
+      <c r="A2" s="12">
+        <v>2251478</v>
+      </c>
+      <c r="B2" s="14">
+        <v>381391</v>
+      </c>
+      <c r="C2" s="14">
+        <v>10</v>
       </c>
       <c r="D2" s="11">
         <v>0</v>
       </c>
-      <c r="E2" s="4">
-        <v>3.5</v>
+      <c r="E2" s="14">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>2139356</v>
-      </c>
-      <c r="B3" s="2">
-        <v>10923</v>
-      </c>
-      <c r="C3" s="4">
-        <v>7</v>
+      <c r="A3" s="13">
+        <v>2315410</v>
+      </c>
+      <c r="B3" s="15">
+        <v>914990</v>
+      </c>
+      <c r="C3" s="15">
+        <v>10</v>
       </c>
       <c r="D3" s="11">
         <v>0</v>
       </c>
-      <c r="E3" s="4">
-        <v>3.5</v>
+      <c r="E3" s="15">
+        <v>13.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>2139501</v>
-      </c>
-      <c r="B4" s="2">
-        <v>75009</v>
-      </c>
-      <c r="C4" s="4">
-        <v>7</v>
+      <c r="A4" s="12">
+        <v>2352005</v>
+      </c>
+      <c r="B4" s="14">
+        <v>25389</v>
+      </c>
+      <c r="C4" s="14">
+        <v>3</v>
       </c>
       <c r="D4" s="11">
         <v>0</v>
       </c>
-      <c r="E4" s="4">
-        <v>3.5</v>
+      <c r="E4" s="14">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>2139488</v>
-      </c>
-      <c r="B5" s="2">
-        <v>36481</v>
-      </c>
-      <c r="C5" s="4">
-        <v>7</v>
+      <c r="A5" s="13">
+        <v>2352260</v>
+      </c>
+      <c r="B5" s="15">
+        <v>69890</v>
+      </c>
+      <c r="C5" s="15">
+        <v>3</v>
       </c>
       <c r="D5" s="11">
         <v>0</v>
       </c>
-      <c r="E5" s="4">
-        <v>3.5</v>
+      <c r="E5" s="15">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>2144308</v>
-      </c>
-      <c r="B6" s="2">
-        <v>85441</v>
-      </c>
-      <c r="C6" s="4">
-        <v>7</v>
+      <c r="A6" s="12">
+        <v>2357726</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1078445</v>
+      </c>
+      <c r="C6" s="14">
+        <v>10</v>
       </c>
       <c r="D6" s="11">
         <v>0</v>
       </c>
-      <c r="E6" s="4">
-        <v>3.5</v>
+      <c r="E6" s="14">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>2148257</v>
-      </c>
-      <c r="B7" s="2">
-        <v>48872</v>
-      </c>
-      <c r="C7" s="4">
-        <v>7</v>
+      <c r="A7" s="13">
+        <v>2361063</v>
+      </c>
+      <c r="B7" s="15">
+        <v>313000</v>
+      </c>
+      <c r="C7" s="15">
+        <v>10</v>
       </c>
       <c r="D7" s="11">
         <v>0</v>
       </c>
-      <c r="E7" s="4">
-        <v>3.5</v>
+      <c r="E7" s="15">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>2151742</v>
-      </c>
-      <c r="B8" s="2">
-        <v>34358</v>
-      </c>
-      <c r="C8" s="4">
-        <v>7</v>
+      <c r="A8" s="12">
+        <v>2361085</v>
+      </c>
+      <c r="B8" s="14">
+        <v>29779</v>
+      </c>
+      <c r="C8" s="14">
+        <v>10</v>
       </c>
       <c r="D8" s="11">
         <v>0</v>
       </c>
-      <c r="E8" s="4">
-        <v>3.5</v>
+      <c r="E8" s="14">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <v>2148308</v>
-      </c>
-      <c r="B9" s="2">
-        <v>76420</v>
-      </c>
-      <c r="C9" s="4">
-        <v>7</v>
+      <c r="A9" s="13">
+        <v>2362421</v>
+      </c>
+      <c r="B9" s="15">
+        <v>84989</v>
+      </c>
+      <c r="C9" s="15">
+        <v>10</v>
       </c>
       <c r="D9" s="11">
         <v>0</v>
       </c>
-      <c r="E9" s="4">
-        <v>3.5</v>
+      <c r="E9" s="15">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>2148170</v>
-      </c>
-      <c r="B10" s="2">
-        <v>18692</v>
-      </c>
-      <c r="C10" s="4">
-        <v>7</v>
+      <c r="A10" s="12">
+        <v>2364838</v>
+      </c>
+      <c r="B10" s="14">
+        <v>44200</v>
+      </c>
+      <c r="C10" s="14">
+        <v>10</v>
       </c>
       <c r="D10" s="11">
         <v>0</v>
       </c>
-      <c r="E10" s="4">
-        <v>3.5</v>
+      <c r="E10" s="14">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>2156807</v>
-      </c>
-      <c r="B11" s="2">
-        <v>23004</v>
-      </c>
-      <c r="C11" s="4">
-        <v>7</v>
+      <c r="A11" s="13">
+        <v>2365215</v>
+      </c>
+      <c r="B11" s="15">
+        <v>167989</v>
+      </c>
+      <c r="C11" s="15">
+        <v>10</v>
       </c>
       <c r="D11" s="11">
         <v>0</v>
       </c>
-      <c r="E11" s="4">
-        <v>3.5</v>
+      <c r="E11" s="15">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>2168452</v>
-      </c>
-      <c r="B12" s="2">
-        <v>21642</v>
-      </c>
-      <c r="C12" s="4">
-        <v>7</v>
+      <c r="A12" s="12">
+        <v>2366128</v>
+      </c>
+      <c r="B12" s="14">
+        <v>119978</v>
+      </c>
+      <c r="C12" s="14">
+        <v>10</v>
       </c>
       <c r="D12" s="11">
         <v>0</v>
       </c>
-      <c r="E12" s="4">
-        <v>3.5</v>
+      <c r="E12" s="14">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <v>2172791</v>
-      </c>
-      <c r="B13" s="2">
-        <v>41602</v>
-      </c>
-      <c r="C13" s="4">
-        <v>7</v>
+      <c r="A13" s="13">
+        <v>2366413</v>
+      </c>
+      <c r="B13" s="15">
+        <v>199989</v>
+      </c>
+      <c r="C13" s="15">
+        <v>10</v>
       </c>
       <c r="D13" s="11">
         <v>0</v>
       </c>
-      <c r="E13" s="4">
-        <v>3.5</v>
+      <c r="E13" s="15">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>2177474</v>
-      </c>
-      <c r="B14" s="2">
-        <v>47070</v>
-      </c>
-      <c r="C14" s="4">
-        <v>7</v>
+      <c r="A14" s="12">
+        <v>2367590</v>
+      </c>
+      <c r="B14" s="14">
+        <v>155000</v>
+      </c>
+      <c r="C14" s="14">
+        <v>10</v>
       </c>
       <c r="D14" s="11">
         <v>0</v>
       </c>
-      <c r="E14" s="4">
-        <v>3.5</v>
+      <c r="E14" s="14">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>2177546</v>
-      </c>
-      <c r="B15" s="2">
-        <v>32592</v>
-      </c>
-      <c r="C15" s="4">
-        <v>7</v>
+      <c r="A15" s="13">
+        <v>2367629</v>
+      </c>
+      <c r="B15" s="15">
+        <v>249989</v>
+      </c>
+      <c r="C15" s="15">
+        <v>10</v>
       </c>
       <c r="D15" s="11">
         <v>0</v>
       </c>
-      <c r="E15" s="4">
-        <v>3.5</v>
+      <c r="E15" s="15">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>2177660</v>
-      </c>
-      <c r="B16" s="2">
-        <v>29380</v>
-      </c>
-      <c r="C16" s="4">
-        <v>7</v>
+      <c r="A16" s="12">
+        <v>2367645</v>
+      </c>
+      <c r="B16" s="14">
+        <v>143989</v>
+      </c>
+      <c r="C16" s="14">
+        <v>16</v>
       </c>
       <c r="D16" s="11">
         <v>0</v>
       </c>
-      <c r="E16" s="4">
-        <v>3.5</v>
+      <c r="E16" s="14">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>2181486</v>
-      </c>
-      <c r="B17" s="2">
-        <v>173228</v>
-      </c>
-      <c r="C17" s="4">
-        <v>7</v>
-      </c>
-      <c r="D17" s="11">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4">
-        <v>3.5</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>2181539</v>
-      </c>
-      <c r="B18" s="2">
-        <v>287111</v>
-      </c>
-      <c r="C18" s="4">
-        <v>7</v>
-      </c>
-      <c r="D18" s="11">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4">
-        <v>3.5</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <v>2188401</v>
-      </c>
-      <c r="B19" s="2">
-        <v>18469</v>
-      </c>
-      <c r="C19" s="4">
-        <v>7</v>
-      </c>
-      <c r="D19" s="11">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4">
-        <v>3.5</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <v>2192199</v>
-      </c>
-      <c r="B20" s="2">
-        <v>66738</v>
-      </c>
-      <c r="C20" s="4">
-        <v>7</v>
-      </c>
-      <c r="D20" s="11">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4">
-        <v>3.5</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <v>2195478</v>
-      </c>
-      <c r="B21" s="2">
-        <v>92084</v>
-      </c>
-      <c r="C21" s="4">
-        <v>7</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0</v>
-      </c>
-      <c r="E21" s="4">
-        <v>3.5</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <v>2202091</v>
-      </c>
-      <c r="B22" s="2">
-        <v>36463</v>
-      </c>
-      <c r="C22" s="4">
-        <v>7</v>
-      </c>
-      <c r="D22" s="11">
-        <v>0</v>
-      </c>
-      <c r="E22" s="4">
-        <v>3.5</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <v>2220684</v>
-      </c>
-      <c r="B23" s="2">
-        <v>62534</v>
-      </c>
-      <c r="C23" s="4">
-        <v>7</v>
-      </c>
-      <c r="D23" s="11">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4">
-        <v>3.5</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
-        <v>2242083</v>
-      </c>
-      <c r="B24" s="2">
-        <v>141501</v>
-      </c>
-      <c r="C24" s="4">
-        <v>7</v>
-      </c>
-      <c r="D24" s="11">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4">
-        <v>3.5</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <v>2239994</v>
-      </c>
-      <c r="B25" s="2">
-        <v>11133</v>
-      </c>
-      <c r="C25" s="4">
-        <v>7</v>
-      </c>
-      <c r="D25" s="11">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4">
-        <v>3.5</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
-        <v>2238666</v>
-      </c>
-      <c r="B26" s="2">
-        <v>17343</v>
-      </c>
-      <c r="C26" s="4">
-        <v>7</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4">
-        <v>3.5</v>
-      </c>
+      <c r="A26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
@@ -1575,7 +1490,7 @@
       <c r="E102" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A5">
+  <conditionalFormatting sqref="A2:A9">
     <cfRule type="duplicateValues" dxfId="9" priority="1"/>
     <cfRule type="duplicateValues" dxfId="8" priority="2"/>
     <cfRule type="duplicateValues" dxfId="7" priority="3"/>
@@ -1587,6 +1502,9 @@
     <cfRule type="duplicateValues" dxfId="1" priority="9"/>
     <cfRule type="duplicateValues" dxfId="0" priority="10"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1" display="https://brokerage24.kz/api/admin/credits/creditapplication/1678366/change/?_changelist_filters=q%3D990419401334%26created_at__year%3D2025" xr:uid="{ADB72A2F-1387-6F4F-AD29-4DC40885D834}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
ozon fixes 15.01.2026 part 3
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADACB42-B649-A348-B904-D2C5F1FEF194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4821C3CC-EDD8-894A-A1D0-94D80D08CDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="1040" windowWidth="27580" windowHeight="13980" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -603,7 +603,7 @@
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -634,156 +634,86 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
-        <v>2264511</v>
+        <v>2310429</v>
       </c>
       <c r="B2" s="14">
-        <v>20121</v>
+        <v>11185</v>
       </c>
       <c r="C2" s="14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" s="14">
         <v>0</v>
       </c>
       <c r="E2" s="14">
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2289214</v>
+        <v>2316494</v>
       </c>
       <c r="B3" s="15">
-        <v>56790</v>
-      </c>
-      <c r="C3" s="15">
+        <v>30605</v>
+      </c>
+      <c r="C3" s="14">
         <v>7</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>0</v>
       </c>
-      <c r="E3" s="15">
-        <v>7.5</v>
+      <c r="E3" s="14">
+        <v>3.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2336118</v>
-      </c>
-      <c r="B4" s="14">
-        <v>32413</v>
-      </c>
-      <c r="C4" s="14">
-        <v>12.5</v>
-      </c>
-      <c r="D4" s="14">
-        <v>0</v>
-      </c>
-      <c r="E4" s="14">
-        <v>13</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2341441</v>
-      </c>
-      <c r="B5" s="15">
-        <v>15813</v>
-      </c>
-      <c r="C5" s="15">
-        <v>7</v>
-      </c>
-      <c r="D5" s="15">
-        <v>0</v>
-      </c>
-      <c r="E5" s="15">
-        <v>7.5</v>
-      </c>
+      <c r="A5"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2347983</v>
-      </c>
-      <c r="B6" s="14">
-        <v>28289</v>
-      </c>
-      <c r="C6" s="15">
-        <v>7</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0</v>
-      </c>
-      <c r="E6" s="15">
-        <v>7.5</v>
-      </c>
+      <c r="A6"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2348446</v>
-      </c>
-      <c r="B7" s="15">
-        <v>11582</v>
-      </c>
-      <c r="C7" s="15">
-        <v>7</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0</v>
-      </c>
-      <c r="E7" s="15">
-        <v>7.5</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>2357313</v>
-      </c>
-      <c r="B8" s="14">
-        <v>11036</v>
-      </c>
-      <c r="C8" s="15">
-        <v>7</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="15">
-        <v>7.5</v>
-      </c>
+      <c r="A8"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2362348</v>
-      </c>
-      <c r="B9" s="15">
-        <v>107252</v>
-      </c>
-      <c r="C9" s="15">
-        <v>7</v>
-      </c>
-      <c r="D9" s="15">
-        <v>0</v>
-      </c>
-      <c r="E9" s="15">
-        <v>7.5</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2367671</v>
-      </c>
-      <c r="B10" s="14">
-        <v>47751</v>
-      </c>
-      <c r="C10" s="15">
-        <v>7</v>
-      </c>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="15">
-        <v>7.5</v>
-      </c>
+      <c r="A10"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>

</xml_diff>

<commit_message>
ozon fixes 15.01.2026 part 4
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4821C3CC-EDD8-894A-A1D0-94D80D08CDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253F810D-C819-7E40-9DDA-A9EFD13DDD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="1040" windowWidth="27580" windowHeight="13980" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -603,7 +603,7 @@
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -634,10 +634,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
-        <v>2310429</v>
+        <v>2305722</v>
       </c>
       <c r="B2" s="14">
-        <v>11185</v>
+        <v>285477</v>
       </c>
       <c r="C2" s="14">
         <v>7</v>
@@ -651,10 +651,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2316494</v>
+        <v>2312187</v>
       </c>
       <c r="B3" s="15">
-        <v>30605</v>
+        <v>27388</v>
       </c>
       <c r="C3" s="14">
         <v>7</v>
@@ -667,32 +667,72 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="A4">
+        <v>2312608</v>
+      </c>
+      <c r="B4" s="14">
+        <v>10723</v>
+      </c>
+      <c r="C4" s="14">
+        <v>7</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="A5">
+        <v>2316491</v>
+      </c>
+      <c r="B5" s="15">
+        <v>23289</v>
+      </c>
+      <c r="C5" s="14">
+        <v>7</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
+      <c r="A6">
+        <v>2319581</v>
+      </c>
+      <c r="B6" s="14">
+        <v>16151</v>
+      </c>
+      <c r="C6" s="14">
+        <v>7</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="A7">
+        <v>2319636</v>
+      </c>
+      <c r="B7" s="15">
+        <v>73757</v>
+      </c>
+      <c r="C7" s="14">
+        <v>7</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0</v>
+      </c>
+      <c r="E7" s="14">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8"/>

</xml_diff>

<commit_message>
wb fixes 29.01.2026 part 2
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C6D228-3022-3B4E-9E46-1DDD1BFB0105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855D4F1B-57BC-8F41-A2CE-44131DE6F0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="1040" windowWidth="27580" windowHeight="13980" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -183,16 +183,115 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -505,7 +604,7 @@
   <dimension ref="A1:E102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -535,11 +634,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>2350821</v>
-      </c>
-      <c r="B2" s="14">
-        <v>19401</v>
+      <c r="A2" s="12">
+        <v>2248847</v>
+      </c>
+      <c r="B2" s="15">
+        <v>62550</v>
       </c>
       <c r="C2" s="14">
         <v>0</v>
@@ -548,15 +647,15 @@
         <v>0</v>
       </c>
       <c r="E2" s="14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2347983</v>
-      </c>
-      <c r="B3" s="15">
-        <v>28289</v>
+      <c r="A3" s="13">
+        <v>2249663</v>
+      </c>
+      <c r="B3" s="16">
+        <v>40570</v>
       </c>
       <c r="C3" s="14">
         <v>0</v>
@@ -565,15 +664,15 @@
         <v>0</v>
       </c>
       <c r="E3" s="14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2357313</v>
-      </c>
-      <c r="B4" s="16">
-        <v>11036</v>
+      <c r="A4" s="12">
+        <v>2251322</v>
+      </c>
+      <c r="B4" s="15">
+        <v>56780</v>
       </c>
       <c r="C4" s="14">
         <v>0</v>
@@ -582,85 +681,195 @@
         <v>0</v>
       </c>
       <c r="E4" s="14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="A5" s="13">
+        <v>2253843</v>
+      </c>
+      <c r="B5" s="16">
+        <v>36770</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="A6" s="12">
+        <v>2251558</v>
+      </c>
+      <c r="B6" s="15">
+        <v>42870</v>
+      </c>
+      <c r="C6" s="14">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="A7" s="13">
+        <v>2256077</v>
+      </c>
+      <c r="B7" s="16">
+        <v>34230</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0</v>
+      </c>
+      <c r="E7" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
+      <c r="A8" s="12">
+        <v>2258086</v>
+      </c>
+      <c r="B8" s="15">
+        <v>26170</v>
+      </c>
+      <c r="C8" s="14">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="A9" s="13">
+        <v>2258381</v>
+      </c>
+      <c r="B9" s="16">
+        <v>19730</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
+      <c r="A10" s="12">
+        <v>2256059</v>
+      </c>
+      <c r="B10" s="15">
+        <v>54780</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0</v>
+      </c>
+      <c r="E10" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="A11" s="13">
+        <v>2260220</v>
+      </c>
+      <c r="B11" s="16">
+        <v>102450</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
+      <c r="E11" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
+      <c r="A12" s="12">
+        <v>2260292</v>
+      </c>
+      <c r="B12" s="15">
+        <v>39020</v>
+      </c>
+      <c r="C12" s="14">
+        <v>0</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0</v>
+      </c>
+      <c r="E12" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
+      <c r="A13" s="13">
+        <v>2260323</v>
+      </c>
+      <c r="B13" s="16">
+        <v>73840</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0</v>
+      </c>
+      <c r="E13" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="A14" s="12">
+        <v>2262116</v>
+      </c>
+      <c r="B14" s="15">
+        <v>43420</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
+      <c r="A15" s="13">
+        <v>2261347</v>
+      </c>
+      <c r="B15" s="16">
+        <v>175480</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0</v>
+      </c>
+      <c r="E15" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
@@ -1272,6 +1481,21 @@
       <c r="E102" s="4"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A9">
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1" display="https://brokerage24.kz/api/admin/credits/creditapplication/1678366/change/?_changelist_filters=q%3D990419401334%26created_at__year%3D2025" xr:uid="{A904960A-77F0-3A41-BF41-5654430F17CA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
ozon fixes part 1 05.02.2026
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855D4F1B-57BC-8F41-A2CE-44131DE6F0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45901C41-E785-6040-9F0C-05A1F78E9043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="1040" windowWidth="27580" windowHeight="13980" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -163,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -180,11 +180,9 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -601,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D67642C-E0A6-4DE4-8C14-031D4C3FE90E}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -634,249 +632,169 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
-        <v>2248847</v>
-      </c>
-      <c r="B2" s="15">
-        <v>62550</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="A2">
+        <v>2500632</v>
+      </c>
+      <c r="B2" s="13">
+        <v>131151</v>
+      </c>
+      <c r="C2" s="12">
+        <v>11.6</v>
+      </c>
+      <c r="D2" s="12">
         <v>0</v>
       </c>
-      <c r="D2" s="14">
+      <c r="E2" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2499894</v>
+      </c>
+      <c r="B3" s="14">
+        <v>294838</v>
+      </c>
+      <c r="C3" s="12">
+        <v>11.6</v>
+      </c>
+      <c r="D3" s="12">
         <v>0</v>
       </c>
-      <c r="E2" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="13">
-        <v>2249663</v>
-      </c>
-      <c r="B3" s="16">
-        <v>40570</v>
-      </c>
-      <c r="C3" s="14">
+      <c r="E3" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2498806</v>
+      </c>
+      <c r="B4" s="13">
+        <v>39399</v>
+      </c>
+      <c r="C4" s="12">
+        <v>11.6</v>
+      </c>
+      <c r="D4" s="12">
         <v>0</v>
       </c>
-      <c r="D3" s="14">
+      <c r="E4" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2498791</v>
+      </c>
+      <c r="B5" s="14">
+        <v>206223</v>
+      </c>
+      <c r="C5" s="12">
+        <v>11.6</v>
+      </c>
+      <c r="D5" s="12">
         <v>0</v>
       </c>
-      <c r="E3" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
-        <v>2251322</v>
-      </c>
-      <c r="B4" s="15">
-        <v>56780</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="E5" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2498590</v>
+      </c>
+      <c r="B6" s="13">
+        <v>204005</v>
+      </c>
+      <c r="C6" s="12">
+        <v>11.6</v>
+      </c>
+      <c r="D6" s="12">
         <v>0</v>
       </c>
-      <c r="D4" s="14">
+      <c r="E6" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2498138</v>
+      </c>
+      <c r="B7" s="14">
+        <v>363541</v>
+      </c>
+      <c r="C7" s="12">
+        <v>11.6</v>
+      </c>
+      <c r="D7" s="12">
         <v>0</v>
       </c>
-      <c r="E4" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="13">
-        <v>2253843</v>
-      </c>
-      <c r="B5" s="16">
-        <v>36770</v>
-      </c>
-      <c r="C5" s="14">
-        <v>0</v>
-      </c>
-      <c r="D5" s="14">
-        <v>0</v>
-      </c>
-      <c r="E5" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
-        <v>2251558</v>
-      </c>
-      <c r="B6" s="15">
-        <v>42870</v>
-      </c>
-      <c r="C6" s="14">
-        <v>0</v>
-      </c>
-      <c r="D6" s="14">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="13">
-        <v>2256077</v>
-      </c>
-      <c r="B7" s="16">
-        <v>34230</v>
-      </c>
-      <c r="C7" s="14">
-        <v>0</v>
-      </c>
-      <c r="D7" s="14">
-        <v>0</v>
-      </c>
-      <c r="E7" s="14">
-        <v>2</v>
+      <c r="E7" s="12">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
-        <v>2258086</v>
-      </c>
-      <c r="B8" s="15">
-        <v>26170</v>
-      </c>
-      <c r="C8" s="14">
-        <v>0</v>
-      </c>
-      <c r="D8" s="14">
-        <v>0</v>
-      </c>
-      <c r="E8" s="14">
-        <v>2</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
-        <v>2258381</v>
-      </c>
-      <c r="B9" s="16">
-        <v>19730</v>
-      </c>
-      <c r="C9" s="14">
-        <v>0</v>
-      </c>
-      <c r="D9" s="14">
-        <v>0</v>
-      </c>
-      <c r="E9" s="14">
-        <v>2</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
-        <v>2256059</v>
-      </c>
-      <c r="B10" s="15">
-        <v>54780</v>
-      </c>
-      <c r="C10" s="14">
-        <v>0</v>
-      </c>
-      <c r="D10" s="14">
-        <v>0</v>
-      </c>
-      <c r="E10" s="14">
-        <v>2</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
-        <v>2260220</v>
-      </c>
-      <c r="B11" s="16">
-        <v>102450</v>
-      </c>
-      <c r="C11" s="14">
-        <v>0</v>
-      </c>
-      <c r="D11" s="14">
-        <v>0</v>
-      </c>
-      <c r="E11" s="14">
-        <v>2</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
-        <v>2260292</v>
-      </c>
-      <c r="B12" s="15">
-        <v>39020</v>
-      </c>
-      <c r="C12" s="14">
-        <v>0</v>
-      </c>
-      <c r="D12" s="14">
-        <v>0</v>
-      </c>
-      <c r="E12" s="14">
-        <v>2</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
-        <v>2260323</v>
-      </c>
-      <c r="B13" s="16">
-        <v>73840</v>
-      </c>
-      <c r="C13" s="14">
-        <v>0</v>
-      </c>
-      <c r="D13" s="14">
-        <v>0</v>
-      </c>
-      <c r="E13" s="14">
-        <v>2</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="12">
-        <v>2262116</v>
-      </c>
-      <c r="B14" s="15">
-        <v>43420</v>
-      </c>
-      <c r="C14" s="14">
-        <v>0</v>
-      </c>
-      <c r="D14" s="14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="14">
-        <v>2</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="13">
-        <v>2261347</v>
-      </c>
-      <c r="B15" s="16">
-        <v>175480</v>
-      </c>
-      <c r="C15" s="14">
-        <v>0</v>
-      </c>
-      <c r="D15" s="14">
-        <v>0</v>
-      </c>
-      <c r="E15" s="14">
-        <v>2</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
@@ -889,63 +807,63 @@
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="11"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="11"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="2"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="11"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="11"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="11"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="2"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="11"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="4"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="11"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="4"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="11"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="2"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="11"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1417,85 +1335,7 @@
       <c r="D93" s="5"/>
       <c r="E93" s="4"/>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A94" s="3"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="5"/>
-      <c r="E94" s="4"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="3"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="5"/>
-      <c r="E95" s="4"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="3"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="4"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" s="3"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="5"/>
-      <c r="E97" s="4"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" s="3"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="4"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="3"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="4"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" s="3"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="4"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101" s="3"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="4"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="4"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="3"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="4"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A9">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
-  </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" display="https://brokerage24.kz/api/admin/credits/creditapplication/1678366/change/?_changelist_filters=q%3D990419401334%26created_at__year%3D2025" xr:uid="{A904960A-77F0-3A41-BF41-5654430F17CA}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
fixes part 1 10.02.2026
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45901C41-E785-6040-9F0C-05A1F78E9043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AD9511-962E-8E4B-A112-A78973D33D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="1040" windowWidth="27580" windowHeight="13980" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -163,7 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -183,6 +188,8 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -599,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D67642C-E0A6-4DE4-8C14-031D4C3FE90E}">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -632,45 +639,45 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>2500632</v>
+      <c r="A2" s="15">
+        <v>2408334</v>
       </c>
       <c r="B2" s="13">
-        <v>131151</v>
+        <v>1016973</v>
       </c>
       <c r="C2" s="12">
-        <v>11.6</v>
+        <v>10</v>
       </c>
       <c r="D2" s="12">
         <v>0</v>
       </c>
       <c r="E2" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2499894</v>
+      <c r="A3" s="15">
+        <v>2418251</v>
       </c>
       <c r="B3" s="14">
-        <v>294838</v>
+        <v>27290</v>
       </c>
       <c r="C3" s="12">
-        <v>11.6</v>
+        <v>3</v>
       </c>
       <c r="D3" s="12">
         <v>0</v>
       </c>
       <c r="E3" s="12">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2498806</v>
+      <c r="A4" s="16">
+        <v>2436829</v>
       </c>
       <c r="B4" s="13">
-        <v>39399</v>
+        <v>554032</v>
       </c>
       <c r="C4" s="12">
         <v>11.6</v>
@@ -679,59 +686,29 @@
         <v>0</v>
       </c>
       <c r="E4" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2498791</v>
-      </c>
-      <c r="B5" s="14">
-        <v>206223</v>
-      </c>
-      <c r="C5" s="12">
-        <v>11.6</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12">
-        <v>12</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2498590</v>
-      </c>
-      <c r="B6" s="13">
-        <v>204005</v>
-      </c>
-      <c r="C6" s="12">
-        <v>11.6</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12">
-        <v>12</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2498138</v>
-      </c>
-      <c r="B7" s="14">
-        <v>363541</v>
-      </c>
-      <c r="C7" s="12">
-        <v>11.6</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12">
-        <v>12</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
@@ -786,21 +763,21 @@
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="11"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1314,28 +1291,19 @@
       <c r="D90" s="5"/>
       <c r="E90" s="4"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" s="3"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="4"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A92" s="3"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="4"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="3"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="4"/>
-    </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A4">
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
fixes part 2 10.02.2026
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AD9511-962E-8E4B-A112-A78973D33D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7033D08C-5B35-2D4B-8D38-20CB729BDF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="1040" windowWidth="27580" windowHeight="13980" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -168,7 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -187,9 +187,7 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -606,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D67642C-E0A6-4DE4-8C14-031D4C3FE90E}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -639,14 +637,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15">
-        <v>2408334</v>
+      <c r="A2" s="14">
+        <v>2508600</v>
       </c>
       <c r="B2" s="13">
-        <v>1016973</v>
+        <v>104989</v>
       </c>
       <c r="C2" s="12">
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="D2" s="12">
         <v>0</v>
@@ -656,38 +654,18 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15">
-        <v>2418251</v>
-      </c>
-      <c r="B3" s="14">
-        <v>27290</v>
-      </c>
-      <c r="C3" s="12">
-        <v>3</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>7</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
-        <v>2436829</v>
-      </c>
-      <c r="B4" s="13">
-        <v>554032</v>
-      </c>
-      <c r="C4" s="12">
-        <v>11.6</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12">
-        <v>13</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
@@ -749,14 +727,14 @@
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="11"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="11"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1277,32 +1255,18 @@
       <c r="D88" s="5"/>
       <c r="E88" s="4"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A89" s="3"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="4"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A90" s="3"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="4"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A4">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="10"/>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="20"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
fixes part 1 16.02.2026
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7033D08C-5B35-2D4B-8D38-20CB729BDF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473D4113-EDB4-4244-84D8-A7CBD5192FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="1040" windowWidth="27580" windowHeight="13980" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E8" sqref="D8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -638,19 +638,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14">
-        <v>2508600</v>
+        <v>2537629</v>
       </c>
       <c r="B2" s="13">
-        <v>104989</v>
+        <v>219990</v>
       </c>
       <c r="C2" s="12">
-        <v>12.5</v>
+        <v>17</v>
       </c>
       <c r="D2" s="12">
         <v>0</v>
       </c>
       <c r="E2" s="12">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixes part 1 18.02.2026
</commit_message>
<xml_diff>
--- a/ozo.xlsx
+++ b/ozo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABE6FA2-25B7-EF4A-9F1C-94BD252BAFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB904465-D106-D142-95C0-F8AC2F8957B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1040" windowWidth="27580" windowHeight="13980" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
+    <workbookView xWindow="2220" yWindow="1020" windowWidth="27580" windowHeight="13980" xr2:uid="{3F67CEAB-F335-4518-8FB9-94B57CB73016}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -607,7 +607,7 @@
   <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -650,7 +650,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="12">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>